<commit_message>
Structural change, additional data
Changed the directory structure, more closely integrating GDP and
population studies.
</commit_message>
<xml_diff>
--- a/Data/GDP Time Series_Long.xlsx
+++ b/Data/GDP Time Series_Long.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moshe\OneDrive\Active\Papers\ECON\GDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moshe\OneDrive\Active\Papers\ECON\econ_git\Econ\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="0" windowWidth="38385" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25620" yWindow="0" windowWidth="38385" windowHeight="21060" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. Bolt</author>
   </authors>
   <commentList>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,12 +52,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. Bolt</author>
   </authors>
   <commentList>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -78,12 +78,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>J. Bolt</author>
   </authors>
   <commentList>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -804,7 +804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8240,7 +8240,7 @@
     <mergeCell ref="Q1:U1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B249" r:id="rId1"/>
+    <hyperlink ref="B249" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8254,10 +8254,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -15019,7 +15019,7 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B335" r:id="rId1"/>
+    <hyperlink ref="B335" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -15033,11 +15033,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H251"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J251"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15197,7 +15197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>1790</v>
       </c>
@@ -15218,8 +15218,12 @@
         <f xml:space="preserve"> B17/E17</f>
         <v>0.98794704603833239</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J17" s="4">
+        <f xml:space="preserve"> 1/G17</f>
+        <v>1.0122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>1791</v>
       </c>
@@ -15241,7 +15245,7 @@
         <v>0.9879470460383325</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>1792</v>
       </c>
@@ -15263,7 +15267,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>1793</v>
       </c>
@@ -15285,7 +15289,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1794</v>
       </c>
@@ -15307,7 +15311,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>1795</v>
       </c>
@@ -15329,7 +15333,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>1796</v>
       </c>
@@ -15351,7 +15355,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>1797</v>
       </c>
@@ -15373,7 +15377,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>1798</v>
       </c>
@@ -15395,7 +15399,7 @@
         <v>0.98794704603833239</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>1799</v>
       </c>
@@ -15417,7 +15421,7 @@
         <v>0.98794704603833228</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>1800</v>
       </c>
@@ -15445,7 +15449,7 @@
         <v>9.0068701078459171E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>1801</v>
       </c>
@@ -15473,7 +15477,7 @@
         <v>8.9465648636356962E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>1802</v>
       </c>
@@ -15501,7 +15505,7 @@
         <v>8.8712589797896646E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>1803</v>
       </c>
@@ -15529,7 +15533,7 @@
         <v>8.7681958288415254E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>1804</v>
       </c>
@@ -15557,7 +15561,7 @@
         <v>8.6471734917681939E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>1805</v>
       </c>

</xml_diff>